<commit_message>
code saved for pg create tables
</commit_message>
<xml_diff>
--- a/db_feed/new_template_v4.xlsx
+++ b/db_feed/new_template_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\db_feed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513701F5-668E-4C8A-8760-66FEFE256FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC48074-8FC4-43FF-990F-51604D40EAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{F8B411A1-6901-4B9B-966C-09D3D94CB0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Origin" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="428">
   <si>
     <t>Solution Information</t>
   </si>
@@ -1511,12 +1511,6 @@
     <t>Fill info below:</t>
   </si>
   <si>
-    <t>Test #</t>
-  </si>
-  <si>
-    <t>filler text</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1540,6 +1534,9 @@
       </rPr>
       <t xml:space="preserve"> Each excel file is for a single sample. For multiple similar samples, duplicate the file and change only the necessary data. One file = one sample.</t>
     </r>
+  </si>
+  <si>
+    <t>Ossila</t>
   </si>
 </sst>
 </file>
@@ -2116,7 +2113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2227,43 +2224,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2275,34 +2238,12 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2310,39 +2251,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2379,10 +2311,25 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2702,15 +2649,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87527978-2A5B-6545-88F5-0DA220A53CEB}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" style="74" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="9" customWidth="1"/>
     <col min="5" max="5" width="52.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
@@ -2723,7 +2670,7 @@
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="67" t="s">
         <v>305</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -2731,19 +2678,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1">
-      <c r="A2" s="127" t="s">
-        <v>428</v>
-      </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
+      <c r="A2" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2" s="99"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="61"/>
       <c r="B3" s="61"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="15.75">
@@ -2753,8 +2700,8 @@
       <c r="B4" s="61" t="s">
         <v>425</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="15.75">
@@ -2764,8 +2711,8 @@
       <c r="B5" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71" t="b">
+      <c r="C5"/>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
@@ -2776,11 +2723,11 @@
       <c r="A6" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="69" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71" t="b">
+      <c r="C6"/>
+      <c r="D6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2791,24 +2738,24 @@
       <c r="B7" s="49" t="s">
         <v>292</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71" t="b">
+      <c r="C7"/>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="30"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
     </row>
     <row r="9" spans="1:5" ht="15.75">
       <c r="A9" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
     </row>
     <row r="10" spans="1:5" ht="15.75">
       <c r="A10" s="30" t="s">
@@ -2817,17 +2764,17 @@
       <c r="B10" s="25" t="s">
         <v>339</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
     </row>
     <row r="11" spans="1:5" ht="15.75">
       <c r="A11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="15.75">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="78"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15.75">
@@ -2841,8 +2788,8 @@
         <v>51</v>
       </c>
       <c r="B14" s="29"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="71" t="b">
+      <c r="C14" s="66"/>
+      <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -2854,8 +2801,8 @@
         <v>52</v>
       </c>
       <c r="B15" s="29"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="71" t="b">
+      <c r="C15" s="66"/>
+      <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="s">
@@ -2867,8 +2814,8 @@
         <v>53</v>
       </c>
       <c r="B16" s="29"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="71" t="b">
+      <c r="C16" s="66"/>
+      <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2878,16 +2825,16 @@
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="78"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="15.75">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="71" t="s">
         <v>337</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="78"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
@@ -2895,7 +2842,6 @@
       <c r="A19" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="74"/>
     </row>
     <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="30" t="s">
@@ -2904,42 +2850,38 @@
       <c r="B20" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="62" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="D21" s="74"/>
     </row>
     <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="74"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="82" t="s">
+      <c r="A23" s="70" t="s">
         <v>335</v>
       </c>
       <c r="B23" s="11"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>128</v>
       </c>
       <c r="B25" s="27"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71" t="b">
+      <c r="C25"/>
+      <c r="D25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2948,8 +2890,8 @@
         <v>129</v>
       </c>
       <c r="B26" s="27"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71" t="b">
+      <c r="C26"/>
+      <c r="D26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2958,8 +2900,8 @@
         <v>34</v>
       </c>
       <c r="B27" s="27"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71" t="b">
+      <c r="C27"/>
+      <c r="D27" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2968,8 +2910,8 @@
         <v>35</v>
       </c>
       <c r="B28" s="27"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71" t="b">
+      <c r="C28"/>
+      <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="9" t="s">
@@ -2981,8 +2923,8 @@
         <v>37</v>
       </c>
       <c r="B29" s="27"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71" t="b">
+      <c r="C29"/>
+      <c r="D29" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2991,8 +2933,8 @@
         <v>38</v>
       </c>
       <c r="B30" s="27"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71" t="b">
+      <c r="C30"/>
+      <c r="D30" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3001,8 +2943,8 @@
         <v>39</v>
       </c>
       <c r="B31" s="27"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71" t="b">
+      <c r="C31"/>
+      <c r="D31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3011,8 +2953,8 @@
         <v>40</v>
       </c>
       <c r="B32" s="27"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71" t="b">
+      <c r="C32"/>
+      <c r="D32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3021,8 +2963,8 @@
         <v>41</v>
       </c>
       <c r="B33" s="27"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71" t="b">
+      <c r="C33"/>
+      <c r="D33" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3031,8 +2973,8 @@
         <v>42</v>
       </c>
       <c r="B34" s="27"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71" t="b">
+      <c r="C34"/>
+      <c r="D34" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3041,8 +2983,8 @@
         <v>43</v>
       </c>
       <c r="B35" s="27"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71" t="b">
+      <c r="C35"/>
+      <c r="D35" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3051,8 +2993,8 @@
         <v>44</v>
       </c>
       <c r="B36" s="27"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71" t="b">
+      <c r="C36"/>
+      <c r="D36" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3061,8 +3003,8 @@
         <v>45</v>
       </c>
       <c r="B37" s="27"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71" t="b">
+      <c r="C37"/>
+      <c r="D37" t="b">
         <v>1</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -3074,24 +3016,16 @@
         <v>47</v>
       </c>
       <c r="B38" s="29"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="71" t="b">
+      <c r="C38" s="66"/>
+      <c r="D38" t="b">
         <v>1</v>
       </c>
       <c r="E38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="D39" s="74"/>
-    </row>
     <row r="41" spans="1:5" ht="15.75">
-      <c r="A41" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>427</v>
-      </c>
+      <c r="A41" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10">
@@ -3192,10 +3126,10 @@
       <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="36" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="105" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="105"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A3" s="16"/>
@@ -58675,8 +58609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5882D5-D74D-473F-B8FF-8824B9621A3C}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:A49"/>
+    <sheetView topLeftCell="A3" zoomScale="114" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -59273,7 +59207,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -59466,7 +59400,9 @@
       <c r="A20" t="s">
         <v>307</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="33" t="s">
+        <v>427</v>
+      </c>
       <c r="D20" t="b">
         <v>1</v>
       </c>
@@ -59693,7 +59629,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -59715,24 +59651,26 @@
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>305</v>
+      </c>
       <c r="E1" s="6"/>
       <c r="F1" s="32"/>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="130.15" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="78"/>
+      <c r="E2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -59741,7 +59679,7 @@
     <row r="3" spans="1:10" ht="16.5" thickBot="1">
       <c r="A3" s="14"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="78"/>
+      <c r="E3" s="3"/>
       <c r="G3" s="45" t="s">
         <v>157</v>
       </c>
@@ -59750,7 +59688,7 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="82" t="s">
         <v>366</v>
       </c>
       <c r="B4" s="40" t="s">
@@ -59759,10 +59697,10 @@
       <c r="C4" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="75" t="s">
         <v>367</v>
       </c>
-      <c r="E4" s="85"/>
+      <c r="E4" s="7"/>
       <c r="G4" s="45"/>
       <c r="H4" s="45"/>
       <c r="I4" s="3"/>
@@ -59772,13 +59710,11 @@
       <c r="A5" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="71"/>
-      <c r="G5" s="105" t="s">
+      <c r="D5" s="76"/>
+      <c r="G5" s="82" t="s">
         <v>153</v>
       </c>
       <c r="H5" s="40" t="s">
@@ -59787,7 +59723,7 @@
       <c r="I5" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -59798,53 +59734,47 @@
       <c r="B6" s="26">
         <v>1</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="71"/>
+      <c r="D6" s="77"/>
       <c r="G6" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="72" t="s">
         <v>345</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="98"/>
+      <c r="J6" s="76"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="99" t="b">
+      <c r="B7" s="73"/>
+      <c r="D7" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="71"/>
       <c r="G7" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H7" s="26"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="98"/>
+      <c r="J7" s="76"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="71" t="s">
+      <c r="B8" s="15">
+        <v>250</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="99" t="b">
+      <c r="D8" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="71"/>
       <c r="G8" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H8" s="92"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="99" t="b">
+      <c r="H8" s="73"/>
+      <c r="J8" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59852,20 +59782,21 @@
       <c r="A9" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="87" t="s">
+      <c r="B9" s="15">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="99" t="b">
+      <c r="D9" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="86"/>
+      <c r="E9" s="3"/>
       <c r="G9" s="36" t="s">
         <v>363</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="99" t="b">
+      <c r="J9" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59873,19 +59804,20 @@
       <c r="A10" s="36" t="s">
         <v>356</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="87" t="s">
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="99" t="b">
+      <c r="D10" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>362</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="99" t="b">
+      <c r="J10" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59895,17 +59827,17 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="47"/>
-      <c r="D11" s="100" t="b">
+      <c r="D11" s="78" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="36" t="s">
         <v>364</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="87" t="s">
+      <c r="I11" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="99" t="b">
+      <c r="J11" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59914,19 +59846,18 @@
         <v>354</v>
       </c>
       <c r="H12" s="42"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="100" t="b">
+      <c r="I12" s="47"/>
+      <c r="J12" s="78" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1">
-      <c r="G13" s="90"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="101"/>
+      <c r="G13" s="22"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="79"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="G14" s="105" t="s">
+      <c r="G14" s="82" t="s">
         <v>366</v>
       </c>
       <c r="H14" s="40" t="s">
@@ -59935,7 +59866,7 @@
       <c r="I14" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J14" s="97" t="s">
+      <c r="J14" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -59943,27 +59874,24 @@
       <c r="G15" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H15" s="89" t="s">
+      <c r="H15" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="I15" s="87"/>
-      <c r="J15" s="98"/>
+      <c r="J15" s="76"/>
     </row>
     <row r="16" spans="1:10">
       <c r="G16" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H16" s="26"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="99"/>
+      <c r="J16" s="77"/>
     </row>
     <row r="17" spans="7:10">
       <c r="G17" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H17" s="92"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="99" t="b">
+      <c r="H17" s="73"/>
+      <c r="J17" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59972,10 +59900,10 @@
         <v>358</v>
       </c>
       <c r="H18" s="15"/>
-      <c r="I18" s="71" t="s">
+      <c r="I18" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="99" t="b">
+      <c r="J18" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59984,10 +59912,10 @@
         <v>355</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="87" t="s">
+      <c r="I19" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="99" t="b">
+      <c r="J19" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -59996,10 +59924,10 @@
         <v>356</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="87" t="s">
+      <c r="I20" t="s">
         <v>158</v>
       </c>
-      <c r="J20" s="99" t="b">
+      <c r="J20" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60009,17 +59937,15 @@
       </c>
       <c r="H21" s="42"/>
       <c r="I21" s="47"/>
-      <c r="J21" s="100" t="b">
+      <c r="J21" s="78" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="7:10" ht="15.75" thickBot="1">
-      <c r="G22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="102"/>
+      <c r="J22" s="80"/>
     </row>
     <row r="23" spans="7:10" ht="15.75">
-      <c r="G23" s="105" t="s">
+      <c r="G23" s="82" t="s">
         <v>154</v>
       </c>
       <c r="H23" s="40" t="s">
@@ -60028,7 +59954,7 @@
       <c r="I23" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="97" t="s">
+      <c r="J23" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -60036,27 +59962,24 @@
       <c r="G24" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H24" s="89" t="s">
+      <c r="H24" s="72" t="s">
         <v>344</v>
       </c>
-      <c r="I24" s="87"/>
-      <c r="J24" s="98"/>
+      <c r="J24" s="76"/>
     </row>
     <row r="25" spans="7:10">
       <c r="G25" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H25" s="26"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="103"/>
+      <c r="J25" s="76"/>
     </row>
     <row r="26" spans="7:10">
       <c r="G26" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H26" s="92"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="99" t="b">
+      <c r="H26" s="73"/>
+      <c r="J26" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60065,10 +59988,10 @@
         <v>348</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="71" t="s">
+      <c r="I27" t="s">
         <v>251</v>
       </c>
-      <c r="J27" s="99" t="b">
+      <c r="J27" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60077,8 +60000,7 @@
         <v>360</v>
       </c>
       <c r="H28" s="15"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="99" t="b">
+      <c r="J28" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60087,8 +60009,7 @@
         <v>351</v>
       </c>
       <c r="H29" s="15"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="99" t="b">
+      <c r="J29" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60097,8 +60018,7 @@
         <v>359</v>
       </c>
       <c r="H30" s="15"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="99" t="b">
+      <c r="J30" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60107,10 +60027,10 @@
         <v>358</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="71" t="s">
+      <c r="I31" t="s">
         <v>21</v>
       </c>
-      <c r="J31" s="99" t="b">
+      <c r="J31" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60119,10 +60039,10 @@
         <v>355</v>
       </c>
       <c r="H32" s="15"/>
-      <c r="I32" s="71" t="s">
+      <c r="I32" t="s">
         <v>23</v>
       </c>
-      <c r="J32" s="99" t="b">
+      <c r="J32" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60131,19 +60051,17 @@
         <v>354</v>
       </c>
       <c r="H33" s="42"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="100" t="b">
+      <c r="I33" s="47"/>
+      <c r="J33" s="78" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="16.5" thickBot="1">
-      <c r="G34" s="88"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="102"/>
+      <c r="G34" s="14"/>
+      <c r="J34" s="80"/>
     </row>
     <row r="35" spans="1:10" ht="15.75">
-      <c r="G35" s="105" t="s">
+      <c r="G35" s="82" t="s">
         <v>155</v>
       </c>
       <c r="H35" s="40" t="s">
@@ -60152,7 +60070,7 @@
       <c r="I35" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J35" s="97" t="s">
+      <c r="J35" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -60160,27 +60078,24 @@
       <c r="G36" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H36" s="93" t="s">
+      <c r="H36" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="I36" s="71"/>
-      <c r="J36" s="103"/>
+      <c r="J36" s="76"/>
     </row>
     <row r="37" spans="1:10">
       <c r="G37" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H37" s="26"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="103"/>
+      <c r="J37" s="76"/>
     </row>
     <row r="38" spans="1:10">
       <c r="G38" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H38" s="92"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="99" t="b">
+      <c r="H38" s="73"/>
+      <c r="J38" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60189,10 +60104,10 @@
         <v>355</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="71" t="s">
+      <c r="I39" t="s">
         <v>23</v>
       </c>
-      <c r="J39" s="99" t="b">
+      <c r="J39" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60201,10 +60116,10 @@
         <v>357</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="71" t="s">
+      <c r="I40" t="s">
         <v>158</v>
       </c>
-      <c r="J40" s="99" t="b">
+      <c r="J40" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60213,16 +60128,16 @@
         <v>354</v>
       </c>
       <c r="H41" s="42"/>
-      <c r="I41" s="95"/>
-      <c r="J41" s="100" t="b">
+      <c r="I41" s="47"/>
+      <c r="J41" s="78" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1">
-      <c r="G42" s="84"/>
-      <c r="H42" s="91"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="104"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="81"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
       <c r="A43" s="2" t="s">
@@ -60231,7 +60146,7 @@
       <c r="B43" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="G43" s="105" t="s">
+      <c r="G43" s="82" t="s">
         <v>156</v>
       </c>
       <c r="H43" s="40" t="s">
@@ -60240,7 +60155,7 @@
       <c r="I43" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J43" s="97" t="s">
+      <c r="J43" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -60248,27 +60163,24 @@
       <c r="G44" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H44" s="89" t="s">
+      <c r="H44" s="72" t="s">
         <v>347</v>
       </c>
-      <c r="I44" s="87"/>
-      <c r="J44" s="98"/>
+      <c r="J44" s="76"/>
     </row>
     <row r="45" spans="1:10">
       <c r="G45" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H45" s="26"/>
-      <c r="I45" s="71"/>
-      <c r="J45" s="103"/>
+      <c r="J45" s="76"/>
     </row>
     <row r="46" spans="1:10">
       <c r="G46" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H46" s="92"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="99" t="b">
+      <c r="H46" s="73"/>
+      <c r="J46" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60277,10 +60189,10 @@
         <v>348</v>
       </c>
       <c r="H47" s="15"/>
-      <c r="I47" s="71" t="s">
+      <c r="I47" t="s">
         <v>251</v>
       </c>
-      <c r="J47" s="99" t="b">
+      <c r="J47" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60289,8 +60201,7 @@
         <v>349</v>
       </c>
       <c r="H48" s="15"/>
-      <c r="I48" s="71"/>
-      <c r="J48" s="99" t="b">
+      <c r="J48" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60299,10 +60210,10 @@
         <v>350</v>
       </c>
       <c r="H49" s="15"/>
-      <c r="I49" s="71" t="s">
+      <c r="I49" t="s">
         <v>159</v>
       </c>
-      <c r="J49" s="99" t="b">
+      <c r="J49" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60311,10 +60222,10 @@
         <v>351</v>
       </c>
       <c r="H50" s="15"/>
-      <c r="I50" s="71" t="s">
+      <c r="I50" t="s">
         <v>160</v>
       </c>
-      <c r="J50" s="99" t="b">
+      <c r="J50" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60323,8 +60234,8 @@
         <v>354</v>
       </c>
       <c r="H51" s="42"/>
-      <c r="I51" s="95"/>
-      <c r="J51" s="100" t="b">
+      <c r="I51" s="47"/>
+      <c r="J51" s="78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60366,8 +60277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FF38F2-F6A4-4E96-86E9-D45968350123}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -60407,139 +60318,149 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="34" t="s">
         <v>368</v>
       </c>
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="B6" s="112">
+      <c r="B6" s="86">
         <v>80</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="87"/>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="B7" s="112">
+      <c r="B7" s="86">
         <v>1500</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="87"/>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="34" t="s">
         <v>372</v>
       </c>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="87" t="s">
         <v>257</v>
       </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="87"/>
+      <c r="C8" s="83"/>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="106"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="106"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="15.75">
       <c r="A11" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="B11" s="110"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="107" t="s">
+      <c r="A12" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="114" t="s">
+      <c r="B13" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="112">
+      <c r="B14" s="86">
         <v>350</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="87"/>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="107" t="s">
+      <c r="A15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
+      <c r="B15" s="87"/>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="107" t="s">
+      <c r="A16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="112"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
+      <c r="B16" s="86"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="B17" s="111"/>
-      <c r="D17" s="87"/>
+      <c r="B17" s="85"/>
     </row>
     <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="B18" s="112"/>
+      <c r="B18" s="86"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="107" t="s">
+      <c r="A19" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="B19" s="112">
+      <c r="B19" s="86">
         <v>0.17199999999999999</v>
       </c>
-      <c r="C19" s="107" t="s">
+      <c r="C19" s="34" t="s">
         <v>26</v>
       </c>
       <c r="D19" t="b">
@@ -60547,11 +60468,11 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="107" t="s">
+      <c r="A20" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="112"/>
-      <c r="C20" s="107" t="s">
+      <c r="B20" s="86"/>
+      <c r="C20" s="34" t="s">
         <v>26</v>
       </c>
       <c r="D20" t="b">
@@ -60562,8 +60483,8 @@
       <c r="A21" t="s">
         <v>376</v>
       </c>
-      <c r="B21" s="112"/>
-      <c r="C21" s="107"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="34"/>
       <c r="D21" t="b">
         <v>1</v>
       </c>
@@ -60572,8 +60493,8 @@
       <c r="A22" t="s">
         <v>377</v>
       </c>
-      <c r="B22" s="112"/>
-      <c r="C22" s="107"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="34"/>
       <c r="D22" t="b">
         <v>1</v>
       </c>
@@ -60582,35 +60503,20 @@
       <c r="A23" t="s">
         <v>378</v>
       </c>
-      <c r="B23" s="112"/>
-      <c r="C23" s="107"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="34"/>
       <c r="D23" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="113"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="D25" s="87"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="D26" s="87"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="D27" s="87"/>
+      <c r="B24" s="85"/>
     </row>
     <row r="28" spans="1:4">
       <c r="D28" s="56"/>
     </row>
-    <row r="29" spans="1:4">
-      <c r="D29" s="87"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="D30" s="87"/>
-    </row>
     <row r="31" spans="1:4">
-      <c r="D31" s="109"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="33" s="1" customFormat="1"/>
     <row r="34" s="1" customFormat="1"/>
@@ -60667,7 +60573,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A46" sqref="A46:B46"/>
     </sheetView>
   </sheetViews>
@@ -60689,19 +60595,19 @@
         <v>305</v>
       </c>
       <c r="E1" s="63"/>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="130.5" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -60722,7 +60628,7 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="G5" s="105" t="s">
+      <c r="G5" s="82" t="s">
         <v>380</v>
       </c>
       <c r="H5" s="40" t="s">
@@ -60731,7 +60637,7 @@
       <c r="I5" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -60739,14 +60645,13 @@
       <c r="G6" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="72" t="s">
         <v>381</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="98"/>
+      <c r="J6" s="76"/>
     </row>
     <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="105" t="s">
+      <c r="A7" s="82" t="s">
         <v>380</v>
       </c>
       <c r="B7" s="40" t="s">
@@ -60755,31 +60660,28 @@
       <c r="C7" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="75" t="s">
         <v>367</v>
       </c>
       <c r="G7" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H7" s="26"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="98"/>
+      <c r="J7" s="76"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="72" t="s">
         <v>381</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="98"/>
+      <c r="D8" s="76"/>
       <c r="G8" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H8" s="92"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="99" t="b">
+      <c r="H8" s="73"/>
+      <c r="J8" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60787,17 +60689,15 @@
       <c r="A9" s="36" t="s">
         <v>353</v>
       </c>
-      <c r="B9" s="114">
+      <c r="B9" s="87">
         <v>1</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="98"/>
+      <c r="D9" s="76"/>
       <c r="G9" s="36" t="s">
         <v>382</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="99" t="b">
+      <c r="J9" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60805,21 +60705,20 @@
       <c r="A10" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="B10" s="125" t="s">
+      <c r="B10" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="99" t="b">
+      <c r="D10" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>355</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="87" t="s">
+      <c r="I10" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="99" t="b">
+      <c r="J10" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60827,11 +60726,10 @@
       <c r="A11" s="36" t="s">
         <v>382</v>
       </c>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="90" t="s">
         <v>421</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="99" t="b">
+      <c r="D11" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="36" t="s">
@@ -60841,7 +60739,7 @@
       <c r="I11" t="s">
         <v>158</v>
       </c>
-      <c r="J11" s="99" t="b">
+      <c r="J11" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60849,21 +60747,21 @@
       <c r="A12" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="117">
+      <c r="B12" s="90">
         <v>25</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="99" t="b">
+      <c r="D12" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="46" t="s">
         <v>354</v>
       </c>
       <c r="H12" s="42"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="100" t="b">
+      <c r="I12" s="47"/>
+      <c r="J12" s="78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60871,30 +60769,29 @@
       <c r="A13" s="36" t="s">
         <v>383</v>
       </c>
-      <c r="B13" s="117">
+      <c r="B13" s="90">
         <v>0.25</v>
       </c>
       <c r="C13" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="99" t="b">
+      <c r="D13" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="101"/>
+      <c r="G13" s="22"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="79"/>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickBot="1">
       <c r="A14" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="B14" s="118"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="100" t="b">
+      <c r="B14" s="91"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="78" t="b">
         <v>1</v>
       </c>
-      <c r="G14" s="105" t="s">
+      <c r="G14" s="82" t="s">
         <v>384</v>
       </c>
       <c r="H14" s="40" t="s">
@@ -60903,7 +60800,7 @@
       <c r="I14" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J14" s="97" t="s">
+      <c r="J14" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -60911,22 +60808,20 @@
       <c r="G15" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H15" s="89" t="s">
+      <c r="H15" s="72" t="s">
         <v>385</v>
       </c>
-      <c r="I15" s="87"/>
-      <c r="J15" s="98"/>
+      <c r="J15" s="76"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="G16" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H16" s="26"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="103"/>
+      <c r="J16" s="76"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="82" t="s">
         <v>384</v>
       </c>
       <c r="B17" s="40" t="s">
@@ -60935,17 +60830,17 @@
       <c r="C17" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="75" t="s">
         <v>367</v>
       </c>
       <c r="G17" s="36" t="s">
         <v>348</v>
       </c>
       <c r="H17" s="15"/>
-      <c r="I17" s="71" t="s">
+      <c r="I17" t="s">
         <v>251</v>
       </c>
-      <c r="J17" s="99" t="b">
+      <c r="J17" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60953,17 +60848,15 @@
       <c r="A18" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B18" s="89" t="s">
+      <c r="B18" s="72" t="s">
         <v>385</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="98"/>
+      <c r="D18" s="76"/>
       <c r="G18" s="36" t="s">
         <v>386</v>
       </c>
       <c r="H18" s="15"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="99" t="b">
+      <c r="J18" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60971,19 +60864,18 @@
       <c r="A19" s="36" t="s">
         <v>353</v>
       </c>
-      <c r="B19" s="114">
+      <c r="B19" s="87">
         <v>2</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="103"/>
+      <c r="D19" s="76"/>
       <c r="G19" s="36" t="s">
         <v>351</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="71" t="s">
+      <c r="I19" t="s">
         <v>160</v>
       </c>
-      <c r="J19" s="99" t="b">
+      <c r="J19" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -60991,21 +60883,21 @@
       <c r="A20" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="B20" s="117">
+      <c r="B20" s="90">
         <v>30</v>
       </c>
-      <c r="C20" s="71" t="s">
+      <c r="C20" t="s">
         <v>251</v>
       </c>
-      <c r="D20" s="99" t="b">
+      <c r="D20" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G20" s="46" t="s">
         <v>354</v>
       </c>
       <c r="H20" s="42"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="100" t="b">
+      <c r="I20" s="47"/>
+      <c r="J20" s="78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61013,9 +60905,8 @@
       <c r="A21" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="99" t="b">
+      <c r="B21" s="90"/>
+      <c r="D21" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61023,14 +60914,14 @@
       <c r="A22" s="36" t="s">
         <v>351</v>
       </c>
-      <c r="B22" s="117"/>
-      <c r="C22" s="71" t="s">
+      <c r="B22" s="90"/>
+      <c r="C22" t="s">
         <v>160</v>
       </c>
-      <c r="D22" s="99" t="b">
+      <c r="D22" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="G22" s="105" t="s">
+      <c r="G22" s="82" t="s">
         <v>387</v>
       </c>
       <c r="H22" s="40" t="s">
@@ -61039,7 +60930,7 @@
       <c r="I22" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J22" s="97" t="s">
+      <c r="J22" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -61047,40 +60938,37 @@
       <c r="A23" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="B23" s="118"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="100" t="b">
+      <c r="B23" s="91"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="78" t="b">
         <v>1</v>
       </c>
       <c r="G23" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H23" s="89" t="s">
+      <c r="H23" s="72" t="s">
         <v>388</v>
       </c>
-      <c r="I23" s="87"/>
-      <c r="J23" s="98"/>
+      <c r="J23" s="76"/>
     </row>
     <row r="24" spans="1:10">
       <c r="G24" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H24" s="26"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="98"/>
+      <c r="J24" s="76"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1">
       <c r="G25" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H25" s="92"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="99" t="b">
+      <c r="H25" s="73"/>
+      <c r="J25" s="77" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75">
-      <c r="A26" s="105" t="s">
+      <c r="A26" s="82" t="s">
         <v>387</v>
       </c>
       <c r="B26" s="40" t="s">
@@ -61089,15 +60977,14 @@
       <c r="C26" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="97" t="s">
+      <c r="D26" s="75" t="s">
         <v>367</v>
       </c>
       <c r="G26" s="36" t="s">
         <v>389</v>
       </c>
       <c r="H26" s="26"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="99" t="b">
+      <c r="J26" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61105,19 +60992,18 @@
       <c r="A27" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="72" t="s">
         <v>388</v>
       </c>
-      <c r="C27" s="87"/>
-      <c r="D27" s="98"/>
+      <c r="D27" s="76"/>
       <c r="G27" s="36" t="s">
         <v>355</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="87" t="s">
+      <c r="I27" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="99" t="b">
+      <c r="J27" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61125,11 +61011,10 @@
       <c r="A28" s="36" t="s">
         <v>353</v>
       </c>
-      <c r="B28" s="114">
+      <c r="B28" s="87">
         <v>3</v>
       </c>
-      <c r="C28" s="87"/>
-      <c r="D28" s="98"/>
+      <c r="D28" s="76"/>
       <c r="G28" s="36" t="s">
         <v>383</v>
       </c>
@@ -61137,7 +61022,7 @@
       <c r="I28" t="s">
         <v>158</v>
       </c>
-      <c r="J28" s="99" t="b">
+      <c r="J28" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61145,19 +61030,18 @@
       <c r="A29" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="B29" s="125" t="s">
+      <c r="B29" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="87"/>
-      <c r="D29" s="99" t="b">
+      <c r="D29" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G29" s="46" t="s">
         <v>354</v>
       </c>
       <c r="H29" s="42"/>
-      <c r="I29" s="95"/>
-      <c r="J29" s="100" t="b">
+      <c r="I29" s="47"/>
+      <c r="J29" s="78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61165,11 +61049,10 @@
       <c r="A30" s="36" t="s">
         <v>389</v>
       </c>
-      <c r="B30" s="114" t="s">
+      <c r="B30" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="87"/>
-      <c r="D30" s="99" t="b">
+      <c r="D30" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61177,16 +61060,16 @@
       <c r="A31" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="B31" s="117">
+      <c r="B31" s="90">
         <v>25</v>
       </c>
-      <c r="C31" s="87" t="s">
+      <c r="C31" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="99" t="b">
+      <c r="D31" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="G31" s="105" t="s">
+      <c r="G31" s="82" t="s">
         <v>172</v>
       </c>
       <c r="H31" s="40" t="s">
@@ -61195,7 +61078,7 @@
       <c r="I31" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J31" s="97" t="s">
+      <c r="J31" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -61203,47 +61086,44 @@
       <c r="A32" s="36" t="s">
         <v>383</v>
       </c>
-      <c r="B32" s="117">
+      <c r="B32" s="90">
         <v>8</v>
       </c>
       <c r="C32" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="99" t="b">
+      <c r="D32" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G32" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H32" s="115" t="s">
+      <c r="H32" s="88" t="s">
         <v>390</v>
       </c>
-      <c r="I32" s="87"/>
-      <c r="J32" s="98"/>
+      <c r="J32" s="76"/>
     </row>
     <row r="33" spans="1:10" ht="16.5" thickBot="1">
       <c r="A33" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="100" t="b">
+      <c r="B33" s="91"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="78" t="b">
         <v>1</v>
       </c>
       <c r="G33" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H33" s="26"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="98"/>
+      <c r="J33" s="76"/>
     </row>
     <row r="34" spans="1:10">
       <c r="G34" s="36" t="s">
         <v>391</v>
       </c>
       <c r="H34" s="15"/>
-      <c r="I34" s="87"/>
-      <c r="J34" s="99" t="b">
+      <c r="J34" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61252,10 +61132,10 @@
         <v>392</v>
       </c>
       <c r="H35" s="15"/>
-      <c r="I35" s="87" t="s">
+      <c r="I35" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="99" t="b">
+      <c r="J35" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61267,7 +61147,7 @@
       <c r="I36" t="s">
         <v>158</v>
       </c>
-      <c r="J36" s="99" t="b">
+      <c r="J36" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61276,8 +61156,8 @@
         <v>354</v>
       </c>
       <c r="H37" s="42"/>
-      <c r="I37" s="95"/>
-      <c r="J37" s="100" t="b">
+      <c r="I37" s="47"/>
+      <c r="J37" s="78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61327,7 +61207,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -61348,20 +61228,23 @@
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="6"/>
-      <c r="F1" s="66" t="s">
+      <c r="D1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F1" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="68"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="93" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="116"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="89"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -61389,9 +61272,7 @@
       <c r="F5" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="40" t="s">
-        <v>147</v>
-      </c>
+      <c r="G5" s="40"/>
       <c r="H5" s="40" t="s">
         <v>148</v>
       </c>
@@ -61403,9 +61284,7 @@
       <c r="A6" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>147</v>
-      </c>
+      <c r="B6" s="40"/>
       <c r="C6" s="40" t="s">
         <v>148</v>
       </c>
@@ -61415,7 +61294,7 @@
       <c r="F6" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="74" t="s">
         <v>399</v>
       </c>
       <c r="I6" s="37"/>
@@ -61424,15 +61303,15 @@
       <c r="A7" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="74" t="s">
         <v>399</v>
       </c>
       <c r="D7" s="37"/>
       <c r="F7" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="G7" s="119"/>
-      <c r="I7" s="96" t="b">
+      <c r="G7" s="92"/>
+      <c r="I7" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61440,20 +61319,20 @@
       <c r="A8" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="92" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="96" t="b">
+      <c r="D8" s="37" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="36" t="s">
         <v>403</v>
       </c>
-      <c r="G8" s="115"/>
+      <c r="G8" s="88"/>
       <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="96" t="b">
+      <c r="I8" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61461,23 +61340,23 @@
       <c r="A9" s="36" t="s">
         <v>403</v>
       </c>
-      <c r="B9" s="115">
+      <c r="B9" s="88">
         <v>1500</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="96" t="b">
+      <c r="D9" s="37" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="36" t="s">
         <v>404</v>
       </c>
-      <c r="G9" s="115"/>
+      <c r="G9" s="88"/>
       <c r="H9" t="s">
         <v>250</v>
       </c>
-      <c r="I9" s="96" t="b">
+      <c r="I9" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61485,23 +61364,23 @@
       <c r="A10" s="36" t="s">
         <v>404</v>
       </c>
-      <c r="B10" s="115">
+      <c r="B10" s="88">
         <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>250</v>
       </c>
-      <c r="D10" s="96" t="b">
+      <c r="D10" s="37" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
         <v>415</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="87" t="s">
+      <c r="H10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="96" t="b">
+      <c r="I10" s="37" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="37" t="s">
@@ -61513,17 +61392,17 @@
         <v>415</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="87" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="96" t="b">
+      <c r="D11" s="37" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="G11" s="115"/>
-      <c r="I11" s="96" t="b">
+      <c r="G11" s="88"/>
+      <c r="I11" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61531,14 +61410,14 @@
       <c r="A12" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="B12" s="115"/>
-      <c r="D12" s="96" t="b">
+      <c r="B12" s="88"/>
+      <c r="D12" s="37" t="b">
         <v>1</v>
       </c>
       <c r="F12" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="G12" s="120"/>
+      <c r="G12" s="93"/>
       <c r="H12" s="50"/>
       <c r="I12" s="43" t="b">
         <v>1</v>
@@ -61548,7 +61427,7 @@
       <c r="A13" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="B13" s="120"/>
+      <c r="B13" s="93"/>
       <c r="C13" s="50"/>
       <c r="D13" s="43" t="b">
         <v>1</v>
@@ -61556,16 +61435,14 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
-      <c r="F14" s="121" t="s">
+      <c r="F14" s="94" t="s">
         <v>169</v>
       </c>
-      <c r="G14" s="122" t="s">
-        <v>151</v>
-      </c>
-      <c r="H14" s="122" t="s">
+      <c r="G14" s="95"/>
+      <c r="H14" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="123" t="s">
+      <c r="I14" s="96" t="s">
         <v>367</v>
       </c>
     </row>
@@ -61573,19 +61450,17 @@
       <c r="F15" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="G15" s="93" t="s">
+      <c r="G15" s="74" t="s">
         <v>402</v>
       </c>
-      <c r="H15" s="71"/>
-      <c r="I15" s="96"/>
+      <c r="I15" s="37"/>
     </row>
     <row r="16" spans="1:10">
       <c r="F16" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="G16" s="124"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="96" t="b">
+      <c r="G16" s="97"/>
+      <c r="I16" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61594,8 +61469,7 @@
         <v>406</v>
       </c>
       <c r="G17" s="15"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="96" t="b">
+      <c r="I17" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61604,8 +61478,7 @@
         <v>407</v>
       </c>
       <c r="G18" s="15"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="96" t="b">
+      <c r="I18" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61614,8 +61487,7 @@
         <v>408</v>
       </c>
       <c r="G19" s="15"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="96" t="b">
+      <c r="I19" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61624,10 +61496,10 @@
         <v>411</v>
       </c>
       <c r="G20" s="15"/>
-      <c r="I20" s="96" t="b">
+      <c r="I20" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="94" t="s">
+      <c r="J20" s="48" t="s">
         <v>269</v>
       </c>
     </row>
@@ -61636,10 +61508,10 @@
         <v>415</v>
       </c>
       <c r="G21" s="15"/>
-      <c r="H21" s="87" t="s">
+      <c r="H21" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="96" t="b">
+      <c r="I21" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61648,10 +61520,10 @@
         <v>409</v>
       </c>
       <c r="G22" s="15"/>
-      <c r="H22" s="71" t="s">
+      <c r="H22" t="s">
         <v>177</v>
       </c>
-      <c r="I22" s="96" t="b">
+      <c r="I22" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61660,8 +61532,7 @@
         <v>412</v>
       </c>
       <c r="G23" s="15"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="96" t="b">
+      <c r="I23" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61670,7 +61541,7 @@
         <v>410</v>
       </c>
       <c r="G24" s="26"/>
-      <c r="I24" s="96" t="b">
+      <c r="I24" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61678,7 +61549,7 @@
       <c r="F25" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="G25" s="120"/>
+      <c r="G25" s="93"/>
       <c r="H25" s="50"/>
       <c r="I25" s="43" t="b">
         <v>1</v>
@@ -61692,9 +61563,7 @@
       <c r="F27" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="G27" s="40" t="s">
-        <v>147</v>
-      </c>
+      <c r="G27" s="40"/>
       <c r="H27" s="40" t="s">
         <v>148</v>
       </c>
@@ -61706,7 +61575,7 @@
       <c r="F28" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="G28" s="93" t="s">
+      <c r="G28" s="74" t="s">
         <v>401</v>
       </c>
       <c r="I28" s="37"/>
@@ -61715,8 +61584,8 @@
       <c r="F29" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="G29" s="119"/>
-      <c r="I29" s="96" t="b">
+      <c r="G29" s="92"/>
+      <c r="I29" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61739,16 +61608,14 @@
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="6:10" ht="15.75">
-      <c r="F32" s="121" t="s">
+      <c r="F32" s="94" t="s">
         <v>418</v>
       </c>
-      <c r="G32" s="122" t="s">
-        <v>151</v>
-      </c>
-      <c r="H32" s="122" t="s">
+      <c r="G32" s="95"/>
+      <c r="H32" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="123" t="s">
+      <c r="I32" s="96" t="s">
         <v>367</v>
       </c>
     </row>
@@ -61756,9 +61623,8 @@
       <c r="F33" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="G33" s="124"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="96"/>
+      <c r="G33" s="97"/>
+      <c r="I33" s="37"/>
       <c r="J33" t="s">
         <v>420</v>
       </c>
@@ -61767,9 +61633,8 @@
       <c r="F34" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="G34" s="124"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="96" t="b">
+      <c r="G34" s="97"/>
+      <c r="I34" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61778,8 +61643,7 @@
         <v>406</v>
       </c>
       <c r="G35" s="15"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="96" t="b">
+      <c r="I35" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61788,10 +61652,10 @@
         <v>415</v>
       </c>
       <c r="G36" s="15"/>
-      <c r="H36" s="87" t="s">
+      <c r="H36" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="96" t="b">
+      <c r="I36" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61800,7 +61664,7 @@
         <v>410</v>
       </c>
       <c r="G37" s="26"/>
-      <c r="I37" s="96" t="b">
+      <c r="I37" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61809,8 +61673,7 @@
         <v>354</v>
       </c>
       <c r="G38" s="15"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="96" t="b">
+      <c r="I38" s="37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -61819,8 +61682,7 @@
         <v>416</v>
       </c>
       <c r="G39" s="38"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="96" t="b">
+      <c r="I39" s="37" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="s">
@@ -61831,7 +61693,7 @@
       <c r="F40" s="44" t="s">
         <v>417</v>
       </c>
-      <c r="G40" s="120"/>
+      <c r="G40" s="93"/>
       <c r="H40" s="50"/>
       <c r="I40" s="43" t="b">
         <v>1</v>
@@ -61842,9 +61704,7 @@
       <c r="F54" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="G54" s="40" t="s">
-        <v>147</v>
-      </c>
+      <c r="G54" s="40"/>
       <c r="H54" s="40" t="s">
         <v>148</v>
       </c>
@@ -61943,19 +61803,19 @@
         <v>305</v>
       </c>
       <c r="E1" s="63"/>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="129.75" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="100" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -61976,7 +61836,7 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="82" t="s">
         <v>396</v>
       </c>
       <c r="B5" s="40" t="s">
@@ -61985,10 +61845,10 @@
       <c r="C5" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="75" t="s">
         <v>367</v>
       </c>
-      <c r="G5" s="105" t="s">
+      <c r="G5" s="82" t="s">
         <v>396</v>
       </c>
       <c r="H5" s="40" t="s">
@@ -61997,7 +61857,7 @@
       <c r="I5" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -62005,49 +61865,43 @@
       <c r="A6" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="72" t="s">
         <v>397</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="98"/>
+      <c r="D6" s="76"/>
       <c r="G6" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="72" t="s">
         <v>397</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="98"/>
+      <c r="J6" s="76"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="36" t="s">
         <v>353</v>
       </c>
       <c r="B7" s="26"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="98"/>
+      <c r="D7" s="76"/>
       <c r="G7" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H7" s="26"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="98"/>
+      <c r="J7" s="76"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="99" t="b">
+      <c r="B8" s="73"/>
+      <c r="D8" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H8" s="92"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="99" t="b">
+      <c r="H8" s="73"/>
+      <c r="J8" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62056,20 +61910,20 @@
         <v>355</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="87" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="99" t="b">
+      <c r="D9" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G9" s="36" t="s">
         <v>355</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="87" t="s">
+      <c r="I9" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="99" t="b">
+      <c r="J9" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62081,7 +61935,7 @@
       <c r="C10" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="99" t="b">
+      <c r="D10" s="77" t="b">
         <v>1</v>
       </c>
       <c r="G10" s="36" t="s">
@@ -62091,7 +61945,7 @@
       <c r="I10" t="s">
         <v>158</v>
       </c>
-      <c r="J10" s="99" t="b">
+      <c r="J10" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62100,27 +61954,26 @@
         <v>354</v>
       </c>
       <c r="B11" s="42"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="100" t="b">
+      <c r="C11" s="47"/>
+      <c r="D11" s="78" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="46" t="s">
         <v>354</v>
       </c>
       <c r="H11" s="42"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="100" t="b">
+      <c r="I11" s="47"/>
+      <c r="J11" s="78" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" thickBot="1">
-      <c r="G12" s="90"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="101"/>
+      <c r="G12" s="22"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="79"/>
     </row>
     <row r="13" spans="1:10" ht="15.75">
-      <c r="G13" s="105" t="s">
+      <c r="G13" s="82" t="s">
         <v>380</v>
       </c>
       <c r="H13" s="40" t="s">
@@ -62129,7 +61982,7 @@
       <c r="I13" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J13" s="97" t="s">
+      <c r="J13" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -62137,27 +61990,24 @@
       <c r="G14" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H14" s="89" t="s">
+      <c r="H14" s="72" t="s">
         <v>381</v>
       </c>
-      <c r="I14" s="87"/>
-      <c r="J14" s="98"/>
+      <c r="J14" s="76"/>
     </row>
     <row r="15" spans="1:10">
       <c r="G15" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H15" s="26"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="98"/>
+      <c r="J15" s="76"/>
     </row>
     <row r="16" spans="1:10">
       <c r="G16" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="H16" s="92"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="99" t="b">
+      <c r="H16" s="73"/>
+      <c r="J16" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62166,8 +62016,7 @@
         <v>382</v>
       </c>
       <c r="H17" s="15"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="99" t="b">
+      <c r="J17" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62176,10 +62025,10 @@
         <v>355</v>
       </c>
       <c r="H18" s="15"/>
-      <c r="I18" s="87" t="s">
+      <c r="I18" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="99" t="b">
+      <c r="J18" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62191,7 +62040,7 @@
       <c r="I19" t="s">
         <v>158</v>
       </c>
-      <c r="J19" s="99" t="b">
+      <c r="J19" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62200,14 +62049,14 @@
         <v>354</v>
       </c>
       <c r="H20" s="42"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="100" t="b">
+      <c r="I20" s="47"/>
+      <c r="J20" s="78" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="7:10" ht="15.75" thickBot="1"/>
     <row r="22" spans="7:10" ht="15.75">
-      <c r="G22" s="105" t="s">
+      <c r="G22" s="82" t="s">
         <v>172</v>
       </c>
       <c r="H22" s="40" t="s">
@@ -62216,7 +62065,7 @@
       <c r="I22" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="J22" s="97" t="s">
+      <c r="J22" s="75" t="s">
         <v>367</v>
       </c>
     </row>
@@ -62224,27 +62073,24 @@
       <c r="G23" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="H23" s="115" t="s">
+      <c r="H23" s="88" t="s">
         <v>390</v>
       </c>
-      <c r="I23" s="87"/>
-      <c r="J23" s="98"/>
+      <c r="J23" s="76"/>
     </row>
     <row r="24" spans="7:10">
       <c r="G24" s="36" t="s">
         <v>353</v>
       </c>
       <c r="H24" s="26"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="98"/>
+      <c r="J24" s="76"/>
     </row>
     <row r="25" spans="7:10">
       <c r="G25" s="36" t="s">
         <v>391</v>
       </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="99" t="b">
+      <c r="J25" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62253,10 +62099,10 @@
         <v>392</v>
       </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="87" t="s">
+      <c r="I26" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="99" t="b">
+      <c r="J26" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62268,7 +62114,7 @@
       <c r="I27" t="s">
         <v>158</v>
       </c>
-      <c r="J27" s="99" t="b">
+      <c r="J27" s="77" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62277,8 +62123,8 @@
         <v>354</v>
       </c>
       <c r="H28" s="42"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="100" t="b">
+      <c r="I28" s="47"/>
+      <c r="J28" s="78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -62342,10 +62188,10 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:7" s="9" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="105"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:7" s="9" customFormat="1" ht="16.899999999999999" customHeight="1">
@@ -62686,11 +62532,11 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" s="9" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
     </row>

</xml_diff>